<commit_message>
fixed issue with commits
</commit_message>
<xml_diff>
--- a/CEI/data/new_CEI.xlsx
+++ b/CEI/data/new_CEI.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H879"/>
+  <dimension ref="A1:H880"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25046,10 +25046,10 @@
         <v>-0.3164548031383833</v>
       </c>
       <c r="E879" t="n">
-        <v>0.2928139546471594</v>
+        <v>0.2999083343810733</v>
       </c>
       <c r="F879" t="n">
-        <v>0.6092687577855427</v>
+        <v>0.6163631375194567</v>
       </c>
       <c r="G879" t="inlineStr">
         <is>
@@ -25058,6 +25058,34 @@
       </c>
       <c r="H879" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B880" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C880" t="n">
+        <v>7</v>
+      </c>
+      <c r="D880" t="n">
+        <v>-0.5544031227900973</v>
+      </c>
+      <c r="E880" t="n">
+        <v>0.6718903117626155</v>
+      </c>
+      <c r="F880" t="n">
+        <v>1.226293434552713</v>
+      </c>
+      <c r="G880" t="inlineStr">
+        <is>
+          <t>NINO3.4 NINO</t>
+        </is>
+      </c>
+      <c r="H880" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>